<commit_message>
Updated fl review --not finished
</commit_message>
<xml_diff>
--- a/AAMC/FL_1_Review.xlsx
+++ b/AAMC/FL_1_Review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melto\Documents\MCAT\AAMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melton\OneDrive\Desktop\MCAT\AAMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07943C9-AF83-4D9C-8ADF-E598B634179A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565AFCCE-FDBC-4C43-A2EA-4BF91966924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChemPhys" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>Flagged</t>
   </si>
@@ -159,9 +159,6 @@
     <t>didn't consider the technology differences… I was thinking orators = hitler or something</t>
   </si>
   <si>
-    <t>??? Shouldve got this wrong… if "peter wronged paul" was the eg</t>
-  </si>
-  <si>
     <t>Bigger issue was that next line was "even if means of communication got better" --&gt; read next paragraph</t>
   </si>
   <si>
@@ -214,13 +211,191 @@
   </si>
   <si>
     <t>I was overthinking again. Had the right answer before…</t>
+  </si>
+  <si>
+    <t>??? Shouldn’t have got this wrong… if "peter wronged paul" was the eg</t>
+  </si>
+  <si>
+    <t>wasn't 100% sure glycolysis made NADH, but now I know</t>
+  </si>
+  <si>
+    <t>Ok got the anatomy of kidney</t>
+  </si>
+  <si>
+    <t>yes, I predicted what the test writer forgot</t>
+  </si>
+  <si>
+    <t>Having nitrogens does not mean it will be polar, which is why I thought it needed active transport</t>
+  </si>
+  <si>
+    <t>reading passage = answer</t>
+  </si>
+  <si>
+    <t>Answer is in the diagram?</t>
+  </si>
+  <si>
+    <t>C doesn't really make sense, b/c the membrane shouldn't let random shit in anyways…</t>
+  </si>
+  <si>
+    <t>I think ok to get wrong…but maybe next time pay more attention to text</t>
+  </si>
+  <si>
+    <t>I forgot that prokaryotic DNA was still double stranded…</t>
+  </si>
+  <si>
+    <r>
+      <t>misinformation effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> occurs when a person's recall of episodic memories becomes less accurate because of post-event information</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>state-dependency effect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> people remember more information if their physical or mental state is the same at time of encoding and time of recall</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dual</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FF5F6368"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>coding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> theory postulates that both visual and verbal information is used to represent information</t>
+    </r>
+  </si>
+  <si>
+    <t>After training, both stimuli and response are called conditioned</t>
+  </si>
+  <si>
+    <t>"I don't go to meetings anymore" --&gt; decreased behavior --&gt; punishment</t>
+  </si>
+  <si>
+    <t>Read the whole paragraph…</t>
+  </si>
+  <si>
+    <r>
+      <t>Affective processes include </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>all feelings and responses, positive or negative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>, related to emotion-laden behavior, knowledge, or beliefs</t>
+    </r>
+  </si>
+  <si>
+    <t>actor-observer bias is a term in social psychology that refers to a tendency to attribute one's own actions to external causes while attributing other people's behaviors to internal causes</t>
+  </si>
+  <si>
+    <t>Optimal arousal theory states that optimal performance requires optimal arousal and that arousal levels that are too high or too low will impede performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skin conductance is caused by sweating </t>
+  </si>
+  <si>
+    <t>parietal lobe = language processing, sensation, perception</t>
+  </si>
+  <si>
+    <t>Selye’s general adaptation syndrome, people’s response to various stressors is similar</t>
+  </si>
+  <si>
+    <t>Question stem had "synchronous" which shouldve indicated cerebellum</t>
+  </si>
+  <si>
+    <t>This was reading comprehension error: they were both doing repetitive behavior</t>
+  </si>
+  <si>
+    <t>Gentrification is the reinvestment in lower income neighborhoods in urban areas, which results from the influx of more affluent groups</t>
+  </si>
+  <si>
+    <t>content gap</t>
+  </si>
+  <si>
+    <r>
+      <t>Nativist theories </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>hypothesize that language is an innate fundamental part of the human genetic make-up</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF202124"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t> and that language acquisition occurs as a natural part of the human experience</t>
+    </r>
+  </si>
+  <si>
+    <t>Sapir–Whorf hypothesis</t>
+  </si>
+  <si>
+    <t>ye so ig sensory memory 1st</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,13 +411,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF4D5156"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF5F6368"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF4D5156"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,16 +495,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -724,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6500457-BB29-4527-B1DF-9BB7B112ABAC}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,110 +1014,110 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>31</v>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -858,47 +1125,47 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>42</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>43</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>45</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>48</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>51</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
+      <c r="B20" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -908,24 +1175,305 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729A98EE-0A1C-4F32-9E56-260E1714A643}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="47.453125" customWidth="1"/>
+    <col min="5" max="5" width="51.54296875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0BA617-6DBC-4E18-A9B2-A134A1B57BA6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="61.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>15</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="51.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="64" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="https://www.verywellmind.com/social-psychology-4157177" xr:uid="{BFCF5497-6247-4CA1-BAD8-352C9241C268}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>